<commit_message>
add some Product mannually, add a python code to download image
</commit_message>
<xml_diff>
--- a/EquationRelatedReactant.xlsx
+++ b/EquationRelatedReactant.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="237" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="474" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="原始数据" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,13 +16,14 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">反应物!$A$1:$C$853</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">反应物!$A$1:$C$853</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">反应物!$A$1:$C$853</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5678" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6083" uniqueCount="699">
   <si>
     <t>二氧化碳的工业制取</t>
   </si>
@@ -1130,7 +1131,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1139,7 +1139,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-</t>
     </r>
@@ -1148,7 +1147,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">丁二烯</t>
     </r>
@@ -1157,7 +1155,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -1166,7 +1163,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1175,7 +1171,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -1184,7 +1179,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">加成的反应</t>
     </r>
@@ -1198,7 +1192,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1207,7 +1200,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-</t>
     </r>
@@ -1216,7 +1208,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">丁二烯</t>
     </r>
@@ -1225,7 +1216,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -1234,7 +1224,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1243,7 +1232,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -1252,7 +1240,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">加成的反应</t>
     </r>
@@ -1284,7 +1271,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1293,7 +1279,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-</t>
     </r>
@@ -1302,7 +1287,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">丁二烯加聚的反应</t>
     </r>
@@ -1460,7 +1444,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">丙醇催化氧化的反应</t>
     </r>
@@ -2095,7 +2078,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2104,7 +2086,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">电解水</t>
     </r>
@@ -2118,7 +2099,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2127,7 +2107,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">木炭还原氧化铜</t>
     </r>
@@ -2144,7 +2123,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2153,7 +2131,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">氢气的点燃</t>
     </r>
@@ -2167,7 +2144,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2176,7 +2152,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">氢气的实验室制取</t>
     </r>
@@ -2190,7 +2165,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2199,7 +2173,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">氢气还原氧化铜</t>
     </r>
@@ -2213,7 +2186,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2222,7 +2194,6 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">一氧化碳的实验室制取</t>
     </r>
@@ -2259,6 +2230,156 @@
   </si>
   <si>
     <t>重铬酸钾</t>
+  </si>
+  <si>
+    <t>氯化钾</t>
+  </si>
+  <si>
+    <t>反应方程式</t>
+  </si>
+  <si>
+    <t>http://kb.cs.tsinghua.edu.cn/apihtml/getjpg/172/Figure-0000-1022</t>
+  </si>
+  <si>
+    <t>NH4NO3＝HNO3＋NH3↑ </t>
+  </si>
+  <si>
+    <t>H2S↔H2+S</t>
+  </si>
+  <si>
+    <t>硫酸氢铵</t>
+  </si>
+  <si>
+    <t>高中P83</t>
+  </si>
+  <si>
+    <t>水 </t>
+  </si>
+  <si>
+    <t>磷酸</t>
+  </si>
+  <si>
+    <t>锰酸钾</t>
+  </si>
+  <si>
+    <t>硫酸钙</t>
+  </si>
+  <si>
+    <t>硅酸钙</t>
+  </si>
+  <si>
+    <t>一水合氨</t>
+  </si>
+  <si>
+    <t>氧化汞</t>
+  </si>
+  <si>
+    <t>硫化汞</t>
+  </si>
+  <si>
+    <t>氟化硅</t>
+  </si>
+  <si>
+    <t>氯化硅</t>
+  </si>
+  <si>
+    <t>碳化硅</t>
+  </si>
+  <si>
+    <t>碳酸氢钙</t>
+  </si>
+  <si>
+    <t>三氯化磷</t>
+  </si>
+  <si>
+    <t>三氧化二铁</t>
+  </si>
+  <si>
+    <t>碘化亚铁</t>
+  </si>
+  <si>
+    <t>氯化铜</t>
+  </si>
+  <si>
+    <t>氯化铝</t>
+  </si>
+  <si>
+    <t>硫化铝</t>
+  </si>
+  <si>
+    <t>硫化镁</t>
+  </si>
+  <si>
+    <t>碘化镁</t>
+  </si>
+  <si>
+    <t>硫酸钡</t>
+  </si>
+  <si>
+    <t>乙酰水杨酸钠</t>
+  </si>
+  <si>
+    <t>钙离子</t>
+  </si>
+  <si>
+    <t>氢氧化铁(胶体)</t>
+  </si>
+  <si>
+    <t>次氯酸</t>
+  </si>
+  <si>
+    <t>亚硫酸氢钙</t>
+  </si>
+  <si>
+    <t>亚硫酸氢钠</t>
+  </si>
+  <si>
+    <t>硫氢化钠</t>
+  </si>
+  <si>
+    <t>醋酸铜</t>
+  </si>
+  <si>
+    <t>醋酸镁</t>
+  </si>
+  <si>
+    <t>硝酸钠</t>
+  </si>
+  <si>
+    <t>醋酸钙</t>
+  </si>
+  <si>
+    <t>四氟化硅</t>
+  </si>
+  <si>
+    <t>银单质</t>
+  </si>
+  <si>
+    <t>硝酸亚铁</t>
+  </si>
+  <si>
+    <t>硫酸亚铁</t>
+  </si>
+  <si>
+    <t>硝酸铜</t>
+  </si>
+  <si>
+    <t>硫酸铝</t>
+  </si>
+  <si>
+    <t>醋酸锌</t>
+  </si>
+  <si>
+    <t>氧化锌</t>
+  </si>
+  <si>
+    <t>硝酸锌</t>
+  </si>
+  <si>
+    <t>硫酸锌</t>
+  </si>
+  <si>
+    <t>氯化锌</t>
   </si>
 </sst>
 </file>
@@ -2273,7 +2394,6 @@
       <sz val="10"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2294,15 +2414,38 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFF66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor rgb="FFFFFF99"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2339,7 +2482,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2360,6 +2503,42 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2369,6 +2548,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFF66"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -2383,7 +2622,7 @@
   </sheetPr>
   <dimension ref="A1:B423"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A387" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A387" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A387" activeCellId="0" sqref="A387"/>
     </sheetView>
   </sheetViews>
@@ -5796,7 +6035,7 @@
   </sheetPr>
   <dimension ref="A1:C635"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A605" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A605" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -12700,7 +12939,7 @@
   </sheetPr>
   <dimension ref="A1:C853"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A815" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A815" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A811" activeCellId="0" sqref="A811"/>
     </sheetView>
   </sheetViews>
@@ -22111,10 +22350,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A423"/>
+  <dimension ref="A1:F422"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A204" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C230" activeCellId="0" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -22127,2114 +22366,3327 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>559</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="0" t="s">
+        <v>605</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="8" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B11" s="0" t="s">
+        <v>649</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B13" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="B14" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="15" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>650</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="16" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="B23" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="24" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="B24" s="8" t="s">
+        <v>547</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="25" s="8" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="B25" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="26" s="8" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="B26" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="27" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="B27" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="28" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
         <v>29</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>654</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="29" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>557</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="35" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>657</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>658</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
+      <c r="B56" s="0" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="57" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="12" t="s">
         <v>58</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="58" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="65" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="2" t="s">
+      <c r="B74" s="0" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="75" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="s">
+      <c r="B75" s="13" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="76" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="12" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="s">
+      <c r="B76" s="13" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="77" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="12" t="s">
         <v>78</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="78" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>677</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>677</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>678</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="2" t="s">
         <v>121</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="121" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B121" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>659</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="C139" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="C141" s="0" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="C142" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="C144" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="C150" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="C151" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="C152" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="C153" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C154" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="C155" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="C156" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="C157" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="C158" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="C159" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>685</v>
+      </c>
+      <c r="C160" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="2" t="s">
         <v>164</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="164" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="C164" s="13" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C165" s="0" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="C166" s="0" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>629</v>
+      </c>
+      <c r="C167" s="0" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="C168" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D168" s="0" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="C169" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D169" s="0" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="D170" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="E170" s="0" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="C171" s="0" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="C173" s="0" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D174" s="0" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="C176" s="0" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="C179" s="0" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>676</v>
+      </c>
+      <c r="C180" s="0" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="C181" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D181" s="0" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="C182" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="D182" s="0" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C183" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="D183" s="0" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="C184" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D184" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="C185" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D185" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="C187" s="0" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C188" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D188" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
+      </c>
+      <c r="B189" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="C189" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D189" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="B190" s="0" t="s">
+        <v>649</v>
+      </c>
+      <c r="C190" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D190" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
+      </c>
+      <c r="B191" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C191" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="B192" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="C192" s="0" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="2" t="s">
         <v>194</v>
+      </c>
+      <c r="B193" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="C193" s="0" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="194" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B194" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="C194" s="13" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="C195" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="B196" s="0" t="s">
+        <v>559</v>
+      </c>
+      <c r="C196" s="0" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="C197" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
+      </c>
+      <c r="B198" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="C198" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C199" s="0" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C200" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="C201" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="2" t="s">
         <v>204</v>
+      </c>
+      <c r="B203" s="0" t="s">
+        <v>576</v>
+      </c>
+      <c r="C203" s="0" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="204" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B204" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="C204" s="13" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C205" s="0" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C206" s="0" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C207" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C208" s="0" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
+      </c>
+      <c r="B211" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="C211" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="C212" s="0" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="C213" s="0" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="C214" s="0" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="C215" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+      <c r="B216" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="C216" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="C217" s="0" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="C218" s="0" t="s">
+        <v>689</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
+      </c>
+      <c r="B219" s="0" t="s">
+        <v>559</v>
+      </c>
+      <c r="C219" s="0" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
+      </c>
+      <c r="B220" s="0" t="s">
+        <v>559</v>
+      </c>
+      <c r="C220" s="0" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B221" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="C221" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="B222" s="0" t="s">
+        <v>693</v>
+      </c>
+      <c r="C222" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
+      </c>
+      <c r="B223" s="0" t="s">
+        <v>694</v>
+      </c>
+      <c r="C223" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
+      </c>
+      <c r="B224" s="0" t="s">
+        <v>695</v>
+      </c>
+      <c r="C224" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="B225" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="C225" s="0" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="B226" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="C226" s="0" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="C227" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="2" t="s">
         <v>229</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="C228" s="0" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="229" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B229" s="13" t="s">
+        <v>605</v>
+      </c>
+      <c r="C229" s="13" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="C230" s="0" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A365" s="2" t="s">
         <v>365</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="3" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="3" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="367" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A367" s="3" t="s">
         <v>367</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="2" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="2" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="374" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="3" t="s">
+    <row r="373" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="3" t="s">
         <v>374</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="2" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="423" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="3" t="s">
+    <row r="422" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A422" s="3" t="s">
         <v>423</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add some product , manually
</commit_message>
<xml_diff>
--- a/EquationRelatedReactant.xlsx
+++ b/EquationRelatedReactant.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="474" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="581" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="原始数据" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,13 +17,14 @@
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">反应物!$A$1:$C$853</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">反应物!$A$1:$C$853</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">反应物!$A$1:$C$853</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">反应物!$A$1:$C$853</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6083" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6125" uniqueCount="703">
   <si>
     <t>二氧化碳的工业制取</t>
   </si>
@@ -1131,6 +1132,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1139,6 +1141,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-</t>
     </r>
@@ -1147,6 +1150,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">丁二烯</t>
     </r>
@@ -1155,6 +1159,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -1163,6 +1168,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1171,6 +1177,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -1179,6 +1186,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">加成的反应</t>
     </r>
@@ -1192,6 +1200,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1200,6 +1209,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-</t>
     </r>
@@ -1208,6 +1218,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">丁二烯</t>
     </r>
@@ -1216,6 +1227,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -1224,6 +1236,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1232,6 +1245,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -1240,6 +1254,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">加成的反应</t>
     </r>
@@ -1271,6 +1286,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1279,6 +1295,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-</t>
     </r>
@@ -1287,6 +1304,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">丁二烯加聚的反应</t>
     </r>
@@ -1444,6 +1462,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">丙醇催化氧化的反应</t>
     </r>
@@ -2078,6 +2097,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2086,6 +2106,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">电解水</t>
     </r>
@@ -2099,6 +2120,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2107,6 +2129,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">木炭还原氧化铜</t>
     </r>
@@ -2123,6 +2146,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2131,6 +2155,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">氢气的点燃</t>
     </r>
@@ -2144,6 +2169,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2152,6 +2178,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">氢气的实验室制取</t>
     </r>
@@ -2165,6 +2192,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2173,6 +2201,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">氢气还原氧化铜</t>
     </r>
@@ -2186,6 +2215,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -2194,6 +2224,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">一氧化碳的实验室制取</t>
     </r>
@@ -2241,7 +2272,7 @@
     <t>http://kb.cs.tsinghua.edu.cn/apihtml/getjpg/172/Figure-0000-1022</t>
   </si>
   <si>
-    <t>NH4NO3＝HNO3＋NH3↑ </t>
+    <t>NH4NO3＝HNO3＋NH3↑</t>
   </si>
   <si>
     <t>H2S↔H2+S</t>
@@ -2253,9 +2284,6 @@
     <t>高中P83</t>
   </si>
   <si>
-    <t>水 </t>
-  </si>
-  <si>
     <t>磷酸</t>
   </si>
   <si>
@@ -2380,6 +2408,21 @@
   </si>
   <si>
     <t>氯化锌</t>
+  </si>
+  <si>
+    <t>硫酸镁</t>
+  </si>
+  <si>
+    <t>硫酸钾</t>
+  </si>
+  <si>
+    <t>硫酸锰</t>
+  </si>
+  <si>
+    <t>亚硫酸根离子</t>
+  </si>
+  <si>
+    <t>钡离子</t>
   </si>
 </sst>
 </file>
@@ -2394,6 +2437,7 @@
       <sz val="10"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2414,6 +2458,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -22352,8 +22397,8 @@
   </sheetPr>
   <dimension ref="A1:F422"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A204" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C230" activeCellId="0" sqref="C230"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A225" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D250" activeCellId="0" sqref="D250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -22546,6 +22591,9 @@
       <c r="C16" s="6" t="s">
         <v>504</v>
       </c>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+      <c r="F16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
@@ -22638,7 +22686,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="25" s="8" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
         <v>26</v>
       </c>
@@ -22652,7 +22700,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="26" s="8" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
@@ -22666,7 +22714,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="27" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
@@ -22677,7 +22725,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="28" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
         <v>29</v>
       </c>
@@ -22702,7 +22750,7 @@
         <v>495</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22788,7 +22836,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>437</v>
@@ -22810,7 +22858,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>510</v>
@@ -22848,7 +22896,7 @@
         <v>43</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22959,7 +23007,7 @@
         <v>58</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="58" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23015,7 +23063,7 @@
         <v>65</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="65" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23079,7 +23127,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23087,7 +23135,7 @@
         <v>74</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23103,7 +23151,7 @@
         <v>76</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="76" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23119,7 +23167,7 @@
         <v>78</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="78" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23127,7 +23175,7 @@
         <v>79</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23178,7 +23226,7 @@
         <v>85</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23194,7 +23242,7 @@
         <v>87</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23242,7 +23290,7 @@
         <v>93</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23266,7 +23314,7 @@
         <v>96</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23290,7 +23338,7 @@
         <v>99</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23322,7 +23370,7 @@
         <v>103</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23330,7 +23378,7 @@
         <v>104</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23370,7 +23418,7 @@
         <v>109</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23378,7 +23426,7 @@
         <v>110</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23405,7 +23453,7 @@
         <v>113</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>428</v>
@@ -23416,7 +23464,7 @@
         <v>114</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>428</v>
@@ -23427,7 +23475,7 @@
         <v>115</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>428</v>
@@ -23446,7 +23494,7 @@
         <v>117</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>428</v>
@@ -23479,13 +23527,13 @@
         <v>120</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C119" s="0" t="s">
         <v>431</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23499,7 +23547,7 @@
         <v>431</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
     </row>
     <row r="121" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23518,7 +23566,7 @@
         <v>123</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23529,7 +23577,7 @@
         <v>499</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23537,7 +23585,7 @@
         <v>125</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>428</v>
@@ -23587,7 +23635,7 @@
         <v>439</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23617,7 +23665,7 @@
         <v>132</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23768,7 +23816,7 @@
         <v>146</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23784,7 +23832,7 @@
         <v>148</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C147" s="0" t="s">
         <v>428</v>
@@ -23795,7 +23843,7 @@
         <v>149</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C148" s="0" t="s">
         <v>428</v>
@@ -23806,7 +23854,7 @@
         <v>150</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C149" s="0" t="s">
         <v>428</v>
@@ -23817,7 +23865,7 @@
         <v>151</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C150" s="0" t="s">
         <v>428</v>
@@ -23839,7 +23887,7 @@
         <v>153</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C152" s="0" t="s">
         <v>428</v>
@@ -23894,7 +23942,7 @@
         <v>158</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C157" s="0" t="s">
         <v>428</v>
@@ -23916,7 +23964,7 @@
         <v>160</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C159" s="0" t="s">
         <v>428</v>
@@ -23927,7 +23975,7 @@
         <v>161</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C160" s="0" t="s">
         <v>428</v>
@@ -23984,7 +24032,7 @@
         <v>167</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C166" s="0" t="s">
         <v>438</v>
@@ -24012,7 +24060,7 @@
         <v>437</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24026,7 +24074,7 @@
         <v>437</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24040,7 +24088,7 @@
         <v>467</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
       <c r="E170" s="0" t="s">
         <v>431</v>
@@ -24076,7 +24124,7 @@
         <v>448</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24084,7 +24132,7 @@
         <v>175</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C174" s="0" t="s">
         <v>428</v>
@@ -24101,7 +24149,7 @@
         <v>622</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24153,10 +24201,10 @@
         <v>181</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24170,7 +24218,7 @@
         <v>437</v>
       </c>
       <c r="D181" s="0" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24184,7 +24232,7 @@
         <v>495</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24198,7 +24246,7 @@
         <v>495</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>656</v>
+        <v>428</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24206,7 +24254,7 @@
         <v>185</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C184" s="0" t="s">
         <v>428</v>
@@ -24416,7 +24464,7 @@
         <v>203</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C202" s="0" t="s">
         <v>458</v>
@@ -24526,10 +24574,10 @@
         <v>213</v>
       </c>
       <c r="B212" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="C212" s="0" t="s">
         <v>689</v>
-      </c>
-      <c r="C212" s="0" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24540,7 +24588,7 @@
         <v>465</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24551,7 +24599,7 @@
         <v>465</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24570,7 +24618,7 @@
         <v>217</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C216" s="0" t="s">
         <v>458</v>
@@ -24581,10 +24629,10 @@
         <v>218</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24592,10 +24640,10 @@
         <v>219</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24625,7 +24673,7 @@
         <v>222</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C221" s="0" t="s">
         <v>458</v>
@@ -24636,7 +24684,7 @@
         <v>223</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C222" s="0" t="s">
         <v>458</v>
@@ -24647,7 +24695,7 @@
         <v>224</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C223" s="0" t="s">
         <v>458</v>
@@ -24658,7 +24706,7 @@
         <v>225</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C224" s="0" t="s">
         <v>458</v>
@@ -24669,10 +24717,10 @@
         <v>226</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24680,7 +24728,7 @@
         <v>227</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C226" s="0" t="s">
         <v>465</v>
@@ -24691,7 +24739,7 @@
         <v>228</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C227" s="0" t="s">
         <v>458</v>
@@ -24702,7 +24750,7 @@
         <v>229</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>458</v>
@@ -24724,7 +24772,7 @@
         <v>231</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>458</v>
@@ -24734,100 +24782,226 @@
       <c r="A231" s="2" t="s">
         <v>232</v>
       </c>
+      <c r="B231" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="C231" s="0" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="2" t="s">
         <v>233</v>
       </c>
+      <c r="B232" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="C232" s="0" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="s">
         <v>234</v>
       </c>
+      <c r="B233" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="C233" s="0" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="2" t="s">
+      <c r="B234" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="C234" s="0" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="235" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="7" t="s">
         <v>236</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="s">
         <v>237</v>
       </c>
+      <c r="B236" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="C236" s="0" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
         <v>238</v>
       </c>
+      <c r="B237" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="C237" s="0" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="2" t="s">
+      <c r="B238" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="C238" s="0" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="239" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="7" t="s">
         <v>240</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="C239" s="8" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
         <v>241</v>
       </c>
+      <c r="B240" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="C240" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="2" t="s">
+      <c r="B241" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="C241" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="D241" s="0" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="242" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="7" t="s">
         <v>243</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="C242" s="8" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
         <v>244</v>
       </c>
+      <c r="B243" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="C243" s="0" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
         <v>245</v>
       </c>
+      <c r="B244" s="0" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
         <v>246</v>
       </c>
+      <c r="B245" s="0" t="s">
+        <v>699</v>
+      </c>
+      <c r="C245" s="0" t="s">
+        <v>700</v>
+      </c>
+      <c r="D245" s="0" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
         <v>247</v>
       </c>
+      <c r="B246" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="C246" s="0" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
         <v>248</v>
       </c>
+      <c r="B247" s="0" t="s">
+        <v>594</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
         <v>249</v>
       </c>
+      <c r="B248" s="0" t="s">
+        <v>701</v>
+      </c>
+      <c r="C248" s="0" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="2" t="s">
+      <c r="B249" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="C249" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D249" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="250" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="7" t="s">
         <v>251</v>
+      </c>
+      <c r="B250" s="8" t="s">
+        <v>629</v>
+      </c>
+      <c r="C250" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="D250" s="8" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add some product , 2017年01月14日19:18:19
</commit_message>
<xml_diff>
--- a/EquationRelatedReactant.xlsx
+++ b/EquationRelatedReactant.xlsx
@@ -19,13 +19,14 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">反应物!$A$1:$C$853</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">反应物!$A$1:$C$853</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">反应物!$A$1:$C$853</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">反应物!$A$1:$C$853</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6269" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6409" uniqueCount="753">
   <si>
     <t>二氧化碳的工业制取</t>
   </si>
@@ -2461,6 +2462,149 @@
   <si>
     <t>氢氧化锌</t>
   </si>
+  <si>
+    <t>碳酸氢根离子</t>
+  </si>
+  <si>
+    <t>四氯化硅</t>
+  </si>
+  <si>
+    <t>硝酸铁</t>
+  </si>
+  <si>
+    <t>偏铝酸根</t>
+  </si>
+  <si>
+    <t>镁离子</t>
+  </si>
+  <si>
+    <t>银氨离子</t>
+  </si>
+  <si>
+    <t>亚硫酸铝</t>
+  </si>
+  <si>
+    <t>锰离子</t>
+  </si>
+  <si>
+    <t>2-丙醇</t>
+  </si>
+  <si>
+    <t>乙烷</t>
+  </si>
+  <si>
+    <t>氯乙烯</t>
+  </si>
+  <si>
+    <t>1,1,2,2-四溴乙烷</t>
+  </si>
+  <si>
+    <t>一氯乙烷</t>
+  </si>
+  <si>
+    <t>1，2-二氯乙烷</t>
+  </si>
+  <si>
+    <t>1,2-二溴乙烷</t>
+  </si>
+  <si>
+    <t>环己烷</t>
+  </si>
+  <si>
+    <t>环己醇</t>
+  </si>
+  <si>
+    <t>聚丙烯</t>
+  </si>
+  <si>
+    <t>聚丙烯腈</t>
+  </si>
+  <si>
+    <t>聚乙烯</t>
+  </si>
+  <si>
+    <t>聚四氟乙烯</t>
+  </si>
+  <si>
+    <t>聚异戊二烯</t>
+  </si>
+  <si>
+    <t>聚苯乙烯</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">聚1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">丁二烯</t>
+    </r>
+  </si>
+  <si>
+    <t>乙酸乙酯</t>
+  </si>
+  <si>
+    <t>乙醚</t>
+  </si>
+  <si>
+    <t>一氯甲烷</t>
+  </si>
+  <si>
+    <t>二氯甲烷</t>
+  </si>
+  <si>
+    <t>三氯甲烷</t>
+  </si>
+  <si>
+    <t>四氯化碳</t>
+  </si>
+  <si>
+    <t>2-硝基甲苯</t>
+  </si>
+  <si>
+    <t>4-硝基甲苯</t>
+  </si>
+  <si>
+    <t>2,4,6-三硝基甲苯</t>
+  </si>
+  <si>
+    <t>溴苯</t>
+  </si>
+  <si>
+    <t>硝基苯</t>
+  </si>
+  <si>
+    <t>三硝基苯酚</t>
+  </si>
+  <si>
+    <t>2,4,6-三溴苯酚</t>
+  </si>
+  <si>
+    <t>酚醛树脂</t>
+  </si>
 </sst>
 </file>
 
@@ -2469,7 +2613,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Droid Sans Fallback"/>
@@ -2496,6 +2640,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -22434,8 +22590,8 @@
   </sheetPr>
   <dimension ref="A1:F422"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A304" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C313" activeCellId="0" sqref="C313"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A388" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B396" activeCellId="0" sqref="B396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -25792,26 +25948,62 @@
       <c r="A314" s="2" t="s">
         <v>315</v>
       </c>
+      <c r="B314" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C314" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="D314" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
         <v>316</v>
       </c>
+      <c r="B315" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C315" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D315" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
         <v>317</v>
       </c>
+      <c r="B316" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="C316" s="0" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
         <v>318</v>
       </c>
+      <c r="B317" s="0" t="s">
+        <v>659</v>
+      </c>
+      <c r="C317" s="0" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
         <v>319</v>
       </c>
+      <c r="B318" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C318" s="0" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
@@ -25827,6 +26019,15 @@
       <c r="A321" s="2" t="s">
         <v>322</v>
       </c>
+      <c r="B321" s="0" t="s">
+        <v>716</v>
+      </c>
+      <c r="C321" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="D321" s="0" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
@@ -25837,196 +26038,418 @@
       <c r="A323" s="2" t="s">
         <v>324</v>
       </c>
+      <c r="B323" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="C323" s="0" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
         <v>325</v>
       </c>
+      <c r="B324" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C324" s="0" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
         <v>326</v>
       </c>
+      <c r="B325" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C325" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D325" s="0" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
         <v>327</v>
       </c>
+      <c r="B326" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
         <v>328</v>
       </c>
+      <c r="B327" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="C327" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="D327" s="0" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
         <v>329</v>
       </c>
+      <c r="B328" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="C328" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D328" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
         <v>330</v>
       </c>
+      <c r="B329" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="C329" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="D329" s="0" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
         <v>331</v>
       </c>
+      <c r="B330" s="0" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
         <v>332</v>
       </c>
+      <c r="B331" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="C331" s="0" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
         <v>333</v>
       </c>
+      <c r="B332" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="C332" s="0" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
         <v>334</v>
       </c>
+      <c r="B333" s="0" t="s">
+        <v>629</v>
+      </c>
+      <c r="C333" s="0" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
         <v>335</v>
       </c>
+      <c r="B334" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="C334" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="D334" s="0" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
         <v>336</v>
       </c>
+      <c r="B335" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="C335" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
         <v>337</v>
       </c>
+      <c r="B336" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C336" s="0" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
         <v>338</v>
       </c>
+      <c r="B337" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="C337" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="D337" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
         <v>339</v>
       </c>
+      <c r="B338" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="C338" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D338" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
         <v>340</v>
       </c>
+      <c r="B339" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="C339" s="0" t="s">
+        <v>558</v>
+      </c>
+      <c r="D339" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
         <v>341</v>
       </c>
+      <c r="B340" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="C340" s="0" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
         <v>342</v>
       </c>
+      <c r="B341" s="0" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
         <v>343</v>
       </c>
+      <c r="B342" s="0" t="s">
+        <v>718</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
         <v>344</v>
       </c>
+      <c r="B343" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="C343" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="D343" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
         <v>345</v>
       </c>
+      <c r="B344" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="C344" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
         <v>346</v>
       </c>
+      <c r="B345" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="C345" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="D345" s="0" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
         <v>347</v>
       </c>
+      <c r="B346" s="0" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
         <v>348</v>
       </c>
+      <c r="B347" s="0" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
         <v>349</v>
       </c>
+      <c r="B348" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="C348" s="0" t="s">
+        <v>721</v>
+      </c>
+      <c r="D348" s="0" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
         <v>350</v>
       </c>
+      <c r="B349" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="C349" s="0" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
         <v>351</v>
       </c>
+      <c r="B350" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="C350" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="D350" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
         <v>352</v>
       </c>
+      <c r="B351" s="0" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
         <v>353</v>
       </c>
+      <c r="B352" s="0" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
         <v>354</v>
       </c>
+      <c r="B353" s="0" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
         <v>355</v>
       </c>
+      <c r="B354" s="0" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
         <v>356</v>
       </c>
+      <c r="B355" s="0" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
         <v>357</v>
       </c>
+      <c r="B356" s="0" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
         <v>358</v>
       </c>
+      <c r="B357" s="0" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
         <v>359</v>
       </c>
+      <c r="B358" s="0" t="s">
+        <v>728</v>
+      </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
         <v>360</v>
       </c>
+      <c r="B359" s="0" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="B360" s="0" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
         <v>362</v>
       </c>
+      <c r="B361" s="0" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
@@ -26037,11 +26460,17 @@
       <c r="A363" s="2" t="s">
         <v>364</v>
       </c>
+      <c r="B363" s="0" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
         <v>365</v>
       </c>
+      <c r="B364" s="0" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="365" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="3" t="s">
@@ -26057,36 +26486,57 @@
       <c r="A367" s="2" t="s">
         <v>368</v>
       </c>
+      <c r="B367" s="0" t="s">
+        <v>732</v>
+      </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
         <v>369</v>
       </c>
+      <c r="B368" s="0" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
         <v>370</v>
       </c>
+      <c r="B369" s="0" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
         <v>371</v>
       </c>
+      <c r="B370" s="0" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
         <v>372</v>
       </c>
+      <c r="B371" s="0" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
         <v>373</v>
       </c>
+      <c r="B372" s="0" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="373" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="3" t="s">
         <v>374</v>
       </c>
+      <c r="B373" s="0" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
@@ -26097,6 +26547,12 @@
       <c r="A375" s="2" t="s">
         <v>376</v>
       </c>
+      <c r="B375" s="0" t="s">
+        <v>739</v>
+      </c>
+      <c r="C375" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
@@ -26107,41 +26563,101 @@
       <c r="A377" s="2" t="s">
         <v>378</v>
       </c>
+      <c r="B377" s="0" t="s">
+        <v>739</v>
+      </c>
+      <c r="C377" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
         <v>379</v>
       </c>
+      <c r="B378" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C378" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
         <v>380</v>
       </c>
+      <c r="B379" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C379" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
         <v>381</v>
       </c>
+      <c r="B380" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="C380" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
         <v>382</v>
       </c>
+      <c r="B381" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C381" s="0" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B382" s="0" t="s">
+        <v>741</v>
+      </c>
+      <c r="C382" s="0" t="s">
+        <v>742</v>
+      </c>
+      <c r="D382" s="0" t="s">
+        <v>743</v>
+      </c>
+      <c r="E382" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="F382" s="0" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
         <v>384</v>
+      </c>
+      <c r="B383" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="C383" s="0" t="s">
+        <v>746</v>
+      </c>
+      <c r="D383" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
         <v>385</v>
       </c>
+      <c r="B384" s="0" t="s">
+        <v>747</v>
+      </c>
+      <c r="C384" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
@@ -26152,50 +26668,110 @@
       <c r="A386" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="B386" s="0" t="s">
+        <v>748</v>
+      </c>
+      <c r="C386" s="0" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
         <v>388</v>
       </c>
+      <c r="B387" s="0" t="s">
+        <v>748</v>
+      </c>
+      <c r="C387" s="0" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
         <v>389</v>
       </c>
+      <c r="B388" s="0" t="s">
+        <v>749</v>
+      </c>
+      <c r="C388" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
         <v>390</v>
       </c>
+      <c r="B389" s="0" t="s">
+        <v>750</v>
+      </c>
+      <c r="C389" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
         <v>391</v>
       </c>
+      <c r="B390" s="0" t="s">
+        <v>751</v>
+      </c>
+      <c r="C390" s="0" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
         <v>392</v>
       </c>
+      <c r="B391" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C391" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
         <v>393</v>
       </c>
+      <c r="B392" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C392" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="D392" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
         <v>394</v>
       </c>
+      <c r="B393" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="C393" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
         <v>395</v>
       </c>
+      <c r="B394" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C394" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
         <v>396</v>
+      </c>
+      <c r="B395" s="0" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add some product , 2017年01月14日19:49:43
</commit_message>
<xml_diff>
--- a/EquationRelatedReactant.xlsx
+++ b/EquationRelatedReactant.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6409" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6457" uniqueCount="765">
   <si>
     <t>二氧化碳的工业制取</t>
   </si>
@@ -2604,6 +2604,42 @@
   </si>
   <si>
     <t>酚醛树脂</t>
+  </si>
+  <si>
+    <t>醋酸根离子</t>
+  </si>
+  <si>
+    <t>乙醇钠</t>
+  </si>
+  <si>
+    <t>硬脂酸甘油酯</t>
+  </si>
+  <si>
+    <t>葡萄糖酸钠</t>
+  </si>
+  <si>
+    <t>氧化亚铜</t>
+  </si>
+  <si>
+    <t>反应物还有氢氧化钠</t>
+  </si>
+  <si>
+    <t>己六醇</t>
+  </si>
+  <si>
+    <t>果糖</t>
+  </si>
+  <si>
+    <t>葡糖酸铵</t>
+  </si>
+  <si>
+    <t>高级脂肪酸纳</t>
+  </si>
+  <si>
+    <t>甘油</t>
+  </si>
+  <si>
+    <t>丙醛</t>
   </si>
 </sst>
 </file>
@@ -22590,8 +22626,8 @@
   </sheetPr>
   <dimension ref="A1:F422"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A388" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B396" activeCellId="0" sqref="B396"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A394" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B423" activeCellId="0" sqref="B423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -26778,21 +26814,45 @@
       <c r="A396" s="2" t="s">
         <v>397</v>
       </c>
+      <c r="B396" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C396" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
         <v>398</v>
       </c>
+      <c r="B397" s="0" t="s">
+        <v>753</v>
+      </c>
+      <c r="C397" s="0" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
         <v>399</v>
       </c>
+      <c r="B398" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="C398" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
         <v>400</v>
       </c>
+      <c r="B399" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C399" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
@@ -26803,26 +26863,47 @@
       <c r="A401" s="2" t="s">
         <v>402</v>
       </c>
+      <c r="B401" s="0" t="s">
+        <v>754</v>
+      </c>
+      <c r="C401" s="0" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
         <v>403</v>
       </c>
+      <c r="B402" s="0" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
         <v>404</v>
       </c>
+      <c r="B403" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C403" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
         <v>405</v>
       </c>
+      <c r="B404" s="0" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
         <v>406</v>
       </c>
+      <c r="B405" s="0" t="s">
+        <v>548</v>
+      </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
@@ -26833,80 +26914,179 @@
       <c r="A407" s="2" t="s">
         <v>408</v>
       </c>
+      <c r="B407" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C407" s="0" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
         <v>409</v>
       </c>
+      <c r="B408" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="C408" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="D408" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="E408" s="0" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
         <v>410</v>
       </c>
+      <c r="B409" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="C409" s="0" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
         <v>411</v>
       </c>
+      <c r="B410" s="0" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
         <v>412</v>
       </c>
+      <c r="B411" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C411" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="2" t="s">
+    <row r="413" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A413" s="7" t="s">
         <v>414</v>
+      </c>
+      <c r="B413" s="8" t="s">
+        <v>756</v>
+      </c>
+      <c r="C413" s="8" t="s">
+        <v>757</v>
+      </c>
+      <c r="D413" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="E413" s="8" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
         <v>415</v>
       </c>
+      <c r="B414" s="0" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
         <v>416</v>
       </c>
+      <c r="B415" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C415" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
         <v>417</v>
       </c>
+      <c r="B416" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C416" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
         <v>418</v>
       </c>
+      <c r="B417" s="0" t="s">
+        <v>536</v>
+      </c>
+      <c r="C417" s="0" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
         <v>419</v>
       </c>
+      <c r="B418" s="0" t="s">
+        <v>761</v>
+      </c>
+      <c r="C418" s="0" t="s">
+        <v>688</v>
+      </c>
+      <c r="D418" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="E418" s="0" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
         <v>420</v>
       </c>
+      <c r="B419" s="0" t="s">
+        <v>762</v>
+      </c>
+      <c r="C419" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
         <v>421</v>
       </c>
+      <c r="B420" s="0" t="s">
+        <v>762</v>
+      </c>
+      <c r="C420" s="0" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
         <v>422</v>
       </c>
+      <c r="B421" s="0" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="422" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="3" t="s">
         <v>423</v>
+      </c>
+      <c r="B422" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="C422" s="0" t="s">
+        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>